<commit_message>
fixed problem with auth in queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ReFramework Introduction Demo Project\REFramework\RoboticEnterpriseFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\UiPath\Auto_Transactions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5769DCE-13EF-46A4-A994-B1C961D4F6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA8D70-0EBF-48DD-AE04-B10FAF2C65C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -180,10 +180,10 @@
     <t>UiDemoCredentialName</t>
   </si>
   <si>
-    <t>TransactionQueue</t>
-  </si>
-  <si>
-    <t>C:\Users\Administrator\Desktop\UiDemo.exe</t>
+    <t>TestQueue</t>
+  </si>
+  <si>
+    <t>D:\Документы\UiPath\RoboticEnterpriseFramework\files\UiDemo.exe</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>